<commit_message>
Added small changes to documents
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Planification.xlsx
+++ b/C61/Phase 1/Planification.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD20C9F-394B-44D1-A76A-C73E17A8258B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6D3F4-A52A-4835-AA61-0E6B31D4A8C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plannification" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculation des sprints" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>Nom</t>
   </si>
@@ -96,9 +97,6 @@
     <t>Optionnel</t>
   </si>
   <si>
-    <t>Création fichier NodeJs</t>
-  </si>
-  <si>
     <t>Estimation du temps (Minutes)</t>
   </si>
   <si>
@@ -118,6 +116,105 @@
   </si>
   <si>
     <t>Création home.html</t>
+  </si>
+  <si>
+    <t>Initialisation de la structure</t>
+  </si>
+  <si>
+    <t>Connecter les "routes"</t>
+  </si>
+  <si>
+    <t>Serveur - saveMatch()</t>
+  </si>
+  <si>
+    <t>Serveur - VerifyLogin()</t>
+  </si>
+  <si>
+    <t>Serveur - nextWord()</t>
+  </si>
+  <si>
+    <t>Game - nextWord()</t>
+  </si>
+  <si>
+    <t>Game - calculateCPM()</t>
+  </si>
+  <si>
+    <t>Game - toJSON()</t>
+  </si>
+  <si>
+    <t>Game - CheckErrors()</t>
+  </si>
+  <si>
+    <t>Game - prepareWord()</t>
+  </si>
+  <si>
+    <t>Word - completedWordToString()</t>
+  </si>
+  <si>
+    <t>Word - addInput()</t>
+  </si>
+  <si>
+    <t>Word - removeLastChar()</t>
+  </si>
+  <si>
+    <t>Adventure - spawnEnemy()</t>
+  </si>
+  <si>
+    <t>Adventure - changeBackground()</t>
+  </si>
+  <si>
+    <t>Adventure - playMusic()</t>
+  </si>
+  <si>
+    <t>Entity - move()</t>
+  </si>
+  <si>
+    <t>Entity - stop()</t>
+  </si>
+  <si>
+    <t>Entity - death()</t>
+  </si>
+  <si>
+    <t>Entity - reduceHealth()</t>
+  </si>
+  <si>
+    <t>Entity - tick()</t>
+  </si>
+  <si>
+    <t>index.html style</t>
+  </si>
+  <si>
+    <t>InGame_trad.html style</t>
+  </si>
+  <si>
+    <t>InGame_adventure.html style</t>
+  </si>
+  <si>
+    <t>home.html style</t>
+  </si>
+  <si>
+    <t>Création modèle usager</t>
+  </si>
+  <si>
+    <t>Création modèle word</t>
+  </si>
+  <si>
+    <t>Création modèle partie</t>
+  </si>
+  <si>
+    <t>Trouver les assets</t>
+  </si>
+  <si>
+    <t>Nombre de tâche</t>
+  </si>
+  <si>
+    <t>Difficulté moyenne</t>
+  </si>
+  <si>
+    <t>Temps total requis</t>
+  </si>
+  <si>
+    <t>Création des fichiers csv</t>
   </si>
 </sst>
 </file>
@@ -179,13 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,6 +294,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,9 +310,6 @@
   <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -233,6 +334,9 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -247,12 +351,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:I81" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="4">
-  <autoFilter ref="C12:I81" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:I89" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="C12:I89" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BEB73C37-012B-4855-AD2E-BF3FC3282F6F}" name="No tâche" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BEB73C37-012B-4855-AD2E-BF3FC3282F6F}" name="No tâche" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{9FB5B8D6-EB0F-453F-9F7B-590278B05C91}" name="Titre"/>
-    <tableColumn id="6" xr3:uid="{1E70752F-88D9-4030-A938-450361DD5532}" name="Tâches préalables" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1E70752F-88D9-4030-A938-450361DD5532}" name="Tâches préalables" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{F97670F9-2262-48ED-AA08-62F6F9DE6530}" name="Priorité"/>
     <tableColumn id="8" xr3:uid="{BC349C26-3803-4636-8F9B-94A4C9F5CD7E}" name="Difficulté"/>
     <tableColumn id="9" xr3:uid="{4BB0A79B-2A72-4D99-BAAE-1417C9CAB8ED}" name="Estimation du temps (Minutes)" dataDxfId="0"/>
@@ -559,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
-  <dimension ref="C3:I81"/>
+  <dimension ref="C3:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +686,10 @@
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="8"/>
       <c r="F4" t="s">
         <v>17</v>
       </c>
@@ -622,501 +726,659 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="8"/>
       <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:9" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="3:9" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="5">
+        <v>30</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="5">
+        <v>45</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="5">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5">
+        <v>30</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="5">
+        <v>30</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="5">
+        <v>60</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="5">
+        <v>60</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="5">
+        <v>120</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="5">
+        <v>180</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="5">
+        <v>120</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="5">
         <v>20</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="7">
-        <v>65</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="I27" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="5">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="7">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="5">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="5">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="7">
-        <v>30</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="5">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="7">
-        <v>60</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="5">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="7">
-        <v>120</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="5">
-        <v>6</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="7">
-        <v>180</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="7">
-        <v>120</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="4"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="4"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="4"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="4"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="4"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="4"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H42" s="8"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H43" s="8"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H44" s="8"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H45" s="8"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H46" s="8"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H47" s="8"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="2"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="8"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" s="8"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H52" s="8"/>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H53" s="8"/>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H54" s="8"/>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H57" s="8"/>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H58" s="8"/>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H59" s="8"/>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H60" s="8"/>
-    </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H61" s="8"/>
-    </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H62" s="8"/>
-    </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H63" s="8"/>
-    </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H64" s="8"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="3"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="6"/>
     </row>
     <row r="65" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H65" s="8"/>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H66" s="8"/>
+      <c r="H66" s="6"/>
     </row>
     <row r="67" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H67" s="8"/>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H68" s="8"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H69" s="8"/>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H70" s="8"/>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H71" s="8"/>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H72" s="8"/>
+      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H73" s="8"/>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H74" s="8"/>
+      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H75" s="8"/>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H76" s="8"/>
+      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H77" s="8"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H78" s="8"/>
+      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H79" s="8"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H80" s="8"/>
+      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H81" s="8"/>
+      <c r="H81" s="6"/>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1124,13 +1386,13 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G128" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G136" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
       <formula1>$G$4:$G$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I81" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I89" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
       <formula1>$H$4:$H$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F81" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F89" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
       <formula1>$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -1139,6 +1401,68 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C66ED9-5FA8-4C32-9D10-F6576DB1E330}">
+  <dimension ref="D6:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="10">
+        <f>COUNTIF(Plannification!I13:I89,Plannification!H4)</f>
+        <v>10</v>
+      </c>
+      <c r="G7" s="10">
+        <f>IF(Plannification!G15=Plannification!G4,1,IF(Plannification!G15=Plannification!G5,5,IF(Plannification!G15=Plannification!G6,10,IF(Plannification!G15=Plannification!G7,7.5,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIF(Plannification!I13:I89,Plannification!H5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <f>COUNTIF(Plannification!I13:I89,Plannification!H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added design patterns in conception.mdj
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Planification.xlsx
+++ b/C61/Phase 1/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6D3F4-A52A-4835-AA61-0E6B31D4A8C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121CF75C-313A-467B-8C77-4EDBDEAD82B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>Nom</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>Création des fichiers csv</t>
+  </si>
+  <si>
+    <t>Création controleur Usager</t>
+  </si>
+  <si>
+    <t>Création controleur Partie</t>
+  </si>
+  <si>
+    <t>Création controleur Word</t>
+  </si>
+  <si>
+    <t>Création Factory()</t>
   </si>
 </sst>
 </file>
@@ -294,8 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -303,6 +313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:I89" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="C12:I89" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:I93" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="C12:I93" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{BEB73C37-012B-4855-AD2E-BF3FC3282F6F}" name="No tâche" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{9FB5B8D6-EB0F-453F-9F7B-590278B05C91}" name="Titre"/>
@@ -663,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
-  <dimension ref="C3:I89"/>
+  <dimension ref="C3:I93"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +698,10 @@
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="11"/>
       <c r="F4" t="s">
         <v>17</v>
       </c>
@@ -726,10 +738,10 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="11"/>
       <c r="G7" t="s">
         <v>11</v>
       </c>
@@ -757,41 +769,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:9" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+    <row r="13" spans="3:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="5">
         <v>30</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="3:9" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+    <row r="14" spans="3:9" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="5">
         <v>45</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1045,7 +1057,7 @@
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="D30" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="2"/>
@@ -1056,7 +1068,7 @@
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="2"/>
@@ -1067,7 +1079,7 @@
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="2"/>
@@ -1078,7 +1090,7 @@
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
@@ -1089,7 +1101,7 @@
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
       <c r="D34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
@@ -1100,7 +1112,7 @@
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
       <c r="D35" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
@@ -1111,7 +1123,7 @@
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
       <c r="D36" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2"/>
@@ -1122,7 +1134,7 @@
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
       <c r="D37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="2"/>
@@ -1133,7 +1145,7 @@
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="3"/>
       <c r="D38" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
@@ -1144,7 +1156,7 @@
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2"/>
@@ -1155,7 +1167,7 @@
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="2"/>
@@ -1166,7 +1178,7 @@
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="2"/>
@@ -1177,7 +1189,7 @@
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="2"/>
@@ -1188,7 +1200,7 @@
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
       <c r="D43" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="2"/>
@@ -1199,7 +1211,7 @@
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="2"/>
@@ -1210,7 +1222,7 @@
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
       <c r="D45" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="2"/>
@@ -1221,7 +1233,7 @@
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
       <c r="D46" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="2"/>
@@ -1232,7 +1244,7 @@
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
       <c r="D47" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
@@ -1243,7 +1255,7 @@
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
       <c r="D48" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="2"/>
@@ -1253,7 +1265,9 @@
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -1261,16 +1275,46 @@
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H50" s="6"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="2"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="6"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="2"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="6"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H53" s="6"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="2"/>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="H54" s="6"/>
@@ -1379,6 +1423,18 @@
     </row>
     <row r="89" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H89" s="6"/>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1386,13 +1442,13 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G136" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G140" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
       <formula1>$G$4:$G$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I89" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I93" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
       <formula1>$H$4:$H$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F89" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F93" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
       <formula1>$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -1408,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C66ED9-5FA8-4C32-9D10-F6576DB1E330}">
   <dimension ref="D6:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1433,11 +1489,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="10">
-        <f>COUNTIF(Plannification!I13:I89,Plannification!H4)</f>
+      <c r="F7" s="8">
+        <f>COUNTIF(Plannification!I13:I93,Plannification!H4)</f>
         <v>10</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <f>IF(Plannification!G15=Plannification!G4,1,IF(Plannification!G15=Plannification!G5,5,IF(Plannification!G15=Plannification!G6,10,IF(Plannification!G15=Plannification!G7,7.5,0))))</f>
         <v>1</v>
       </c>
@@ -1447,7 +1503,7 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <f>COUNTIF(Plannification!I13:I89,Plannification!H5)</f>
+        <f>COUNTIF(Plannification!I13:I93,Plannification!H5)</f>
         <v>1</v>
       </c>
     </row>
@@ -1456,7 +1512,7 @@
         <v>16</v>
       </c>
       <c r="F9">
-        <f>COUNTIF(Plannification!I13:I89,Plannification!H6)</f>
+        <f>COUNTIF(Plannification!I13:I93,Plannification!H6)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>